<commit_message>
Added results for Salinas dataset
</commit_message>
<xml_diff>
--- a/IP/results/SummaryIP.xlsx
+++ b/IP/results/SummaryIP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w63x712\Documents\Machine_Learning\HSI_selection2\IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69D67B5-8AB7-4D17-823F-4AACDAE54C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA6BEAE-8A2B-4923-87D3-99F496C0DFE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="4" xr2:uid="{D4E1857A-7969-4B6E-A5E0-8AB94818FDA4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="8" xr2:uid="{D4E1857A-7969-4B6E-A5E0-8AB94818FDA4}"/>
   </bookViews>
   <sheets>
     <sheet name="200 bands" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="461">
   <si>
     <t>SVM</t>
   </si>
@@ -497,9 +497,6 @@
     <t>Method</t>
   </si>
   <si>
-    <t>6 bands</t>
-  </si>
-  <si>
     <t>Original</t>
   </si>
   <si>
@@ -953,9 +950,6 @@
     <t>94.758% (+/- 1.480%)</t>
   </si>
   <si>
-    <t>94.890% (+/- 1.117%)</t>
-  </si>
-  <si>
     <t>93.872% (+/- 0.794%)</t>
   </si>
   <si>
@@ -1016,9 +1010,6 @@
     <t>84.692% (+/- 3.307%)</t>
   </si>
   <si>
-    <t>86.223% (+/- 2.766%)</t>
-  </si>
-  <si>
     <t>87.229% (+/- 1.911%)</t>
   </si>
   <si>
@@ -1428,6 +1419,12 @@
   </si>
   <si>
     <t>87.100% (+/- 2.764%)</t>
+  </si>
+  <si>
+    <t>86.123% (+/- 2.766%)</t>
+  </si>
+  <si>
+    <t>94.490% (+/- 1.117%)</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1464,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1586,10 +1582,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2854,8 +2850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448D17FE-18CC-46F5-BAC3-3C9188DFBB42}">
   <dimension ref="B3:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2903,16 +2899,16 @@
         <v>11</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -2923,16 +2919,16 @@
         <v>52</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -2943,16 +2939,16 @@
         <v>53</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
@@ -2963,16 +2959,16 @@
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
@@ -2983,16 +2979,16 @@
         <v>15</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
@@ -3003,16 +2999,16 @@
         <v>16</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>209</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -3023,16 +3019,16 @@
         <v>63</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
@@ -3043,16 +3039,16 @@
         <v>64</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>217</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -3068,16 +3064,16 @@
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>221</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
@@ -3085,7 +3081,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -3116,16 +3112,16 @@
         <v>11</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="F24" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>253</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -3136,16 +3132,16 @@
         <v>52</v>
       </c>
       <c r="D25" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="F25" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>257</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
@@ -3156,16 +3152,16 @@
         <v>53</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
@@ -3176,16 +3172,16 @@
         <v>14</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>265</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
@@ -3196,16 +3192,16 @@
         <v>15</v>
       </c>
       <c r="D28" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="F28" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>269</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
@@ -3216,16 +3212,16 @@
         <v>16</v>
       </c>
       <c r="D29" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="F29" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="G29" s="9" t="s">
         <v>273</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
@@ -3236,16 +3232,16 @@
         <v>63</v>
       </c>
       <c r="D30" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="F30" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="G30" s="9" t="s">
         <v>277</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
@@ -3256,16 +3252,16 @@
         <v>64</v>
       </c>
       <c r="D31" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="F31" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="G31" s="9" t="s">
         <v>281</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
@@ -3290,7 +3286,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
@@ -3321,36 +3317,36 @@
         <v>11</v>
       </c>
       <c r="D42" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="E42" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="F42" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="F42" s="9" t="s">
+      <c r="G42" s="9" t="s">
         <v>286</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="9">
         <v>11</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="21" t="s">
         <v>52</v>
       </c>
       <c r="D43" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E43" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="F43" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="G43" s="9" t="s">
         <v>290</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
@@ -3361,16 +3357,16 @@
         <v>53</v>
       </c>
       <c r="D44" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
@@ -3381,16 +3377,16 @@
         <v>14</v>
       </c>
       <c r="D45" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
@@ -3401,16 +3397,16 @@
         <v>15</v>
       </c>
       <c r="D46" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="E46" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="F46" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="F46" s="9" t="s">
-        <v>302</v>
-      </c>
       <c r="G46" s="9" t="s">
-        <v>303</v>
+        <v>460</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
@@ -3421,16 +3417,16 @@
         <v>16</v>
       </c>
       <c r="D47" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="F47" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="G47" s="9" t="s">
         <v>305</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
@@ -3441,16 +3437,16 @@
         <v>63</v>
       </c>
       <c r="D48" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="F48" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="G48" s="9" t="s">
         <v>309</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
@@ -3461,16 +3457,16 @@
         <v>64</v>
       </c>
       <c r="D49" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="F49" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="G49" s="9" t="s">
         <v>313</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
@@ -3494,8 +3490,8 @@
       <c r="B57" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="21" t="s">
-        <v>316</v>
+      <c r="C57" s="20" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
@@ -3526,16 +3522,16 @@
         <v>11</v>
       </c>
       <c r="D60" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="F60" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="G60" s="9" t="s">
         <v>318</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
@@ -3546,16 +3542,16 @@
         <v>12</v>
       </c>
       <c r="D61" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="F61" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="E61" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>323</v>
-      </c>
       <c r="G61" s="9" t="s">
-        <v>324</v>
+        <v>459</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
@@ -3566,16 +3562,16 @@
         <v>53</v>
       </c>
       <c r="D62" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
@@ -3586,16 +3582,16 @@
         <v>14</v>
       </c>
       <c r="D63" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>329</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
@@ -3606,16 +3602,16 @@
         <v>15</v>
       </c>
       <c r="D64" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="G64" s="9" t="s">
         <v>333</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
@@ -3626,16 +3622,16 @@
         <v>16</v>
       </c>
       <c r="D65" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="G65" s="9" t="s">
         <v>337</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
@@ -3646,16 +3642,16 @@
         <v>63</v>
       </c>
       <c r="D66" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="G66" s="9" t="s">
         <v>341</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
@@ -3666,16 +3662,16 @@
         <v>64</v>
       </c>
       <c r="D67" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="G67" s="9" t="s">
         <v>345</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
@@ -3711,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D34A67-7EA1-4E46-B651-5814B8ED44C8}">
   <dimension ref="A3:J30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3732,7 +3728,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -3740,7 +3736,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>151</v>
+        <v>51</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
@@ -3771,25 +3767,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>153</v>
-      </c>
       <c r="C7" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="G7" s="24" t="s">
         <v>162</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>163</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="14"/>
@@ -3797,20 +3793,20 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="12" t="s">
         <v>168</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>169</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="25"/>
@@ -3819,25 +3815,25 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>181</v>
-      </c>
       <c r="G9" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="14"/>
@@ -3845,20 +3841,20 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="12" t="s">
         <v>184</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>185</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="25"/>
@@ -3867,25 +3863,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>173</v>
-      </c>
       <c r="G11" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="14"/>
@@ -3893,20 +3889,20 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>177</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="25"/>
@@ -3915,25 +3911,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>236</v>
-      </c>
       <c r="G13" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="14"/>
@@ -3941,20 +3937,20 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>240</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="27"/>
@@ -3963,25 +3959,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="G15" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="15"/>
@@ -3989,20 +3985,20 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="13" t="s">
         <v>244</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>245</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
@@ -4011,10 +4007,10 @@
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D20" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.3">
@@ -4023,34 +4019,34 @@
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D22" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D23" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D24" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D25" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.3">
@@ -4059,34 +4055,34 @@
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D27" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D28" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D29" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D30" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -4115,7 +4111,7 @@
   <dimension ref="A3:J30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C5" sqref="C5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4135,7 +4131,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4143,7 +4139,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>151</v>
+        <v>51</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
@@ -4174,25 +4170,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>153</v>
-      </c>
       <c r="C7" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>381</v>
-      </c>
       <c r="G7" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="14"/>
@@ -4200,20 +4196,20 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>382</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>384</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>385</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="25"/>
@@ -4222,25 +4218,25 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>405</v>
-      </c>
       <c r="G9" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="14"/>
@@ -4248,20 +4244,20 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>406</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>407</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>409</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="25"/>
@@ -4270,25 +4266,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>427</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>428</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>429</v>
-      </c>
       <c r="G11" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="14"/>
@@ -4296,20 +4292,20 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>433</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="25"/>
@@ -4318,25 +4314,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>357</v>
-      </c>
       <c r="G13" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="14"/>
@@ -4344,20 +4340,20 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>358</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>361</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="27"/>
@@ -4366,25 +4362,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>262</v>
-      </c>
       <c r="G15" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="15"/>
@@ -4392,20 +4388,20 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>450</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>451</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>452</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>453</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
@@ -4414,10 +4410,10 @@
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D20" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.3">
@@ -4426,34 +4422,34 @@
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D22" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D23" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D24" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D25" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.3">
@@ -4501,7 +4497,7 @@
   <dimension ref="A3:J30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C5" sqref="C5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4521,7 +4517,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4529,7 +4525,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>151</v>
+        <v>51</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
@@ -4560,25 +4556,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>153</v>
-      </c>
       <c r="C7" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>387</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>389</v>
-      </c>
       <c r="G7" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="14"/>
@@ -4586,20 +4582,20 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>390</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>393</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="25"/>
@@ -4608,25 +4604,25 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>410</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>413</v>
-      </c>
       <c r="G9" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="14"/>
@@ -4634,20 +4630,20 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>414</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>416</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>417</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="25"/>
@@ -4656,25 +4652,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="18" t="s">
+        <v>431</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>433</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>434</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>435</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>436</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>437</v>
-      </c>
       <c r="G11" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="14"/>
@@ -4682,20 +4678,20 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="18" t="s">
+        <v>435</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>436</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>437</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>438</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>439</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>440</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>441</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="25"/>
@@ -4704,25 +4700,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>363</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>365</v>
-      </c>
       <c r="G13" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="14"/>
@@ -4730,20 +4726,20 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>366</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>369</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="27"/>
@@ -4752,25 +4748,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>299</v>
-      </c>
       <c r="G15" s="26" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="15"/>
@@ -4778,20 +4774,20 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>454</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>455</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>457</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
@@ -4800,10 +4796,10 @@
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D20" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.3">
@@ -4812,34 +4808,34 @@
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D22" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D23" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D24" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D25" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.3">
@@ -4886,8 +4882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FC768F-9925-423C-8CB8-7B0AC8AB7AFE}">
   <dimension ref="A3:J30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4907,7 +4903,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4915,7 +4911,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>151</v>
+        <v>51</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
@@ -4946,25 +4942,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>153</v>
-      </c>
       <c r="C7" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>397</v>
-      </c>
       <c r="G7" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="14"/>
@@ -4972,20 +4968,20 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>398</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>401</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="25"/>
@@ -4994,25 +4990,25 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>421</v>
-      </c>
       <c r="G9" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="14"/>
@@ -5020,20 +5016,20 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>422</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>423</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>425</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="25"/>
@@ -5042,25 +5038,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="18" t="s">
+        <v>439</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>443</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>444</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>445</v>
-      </c>
       <c r="G11" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="14"/>
@@ -5068,20 +5064,20 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>444</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>445</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>446</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>447</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>448</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>449</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="25"/>
@@ -5090,25 +5086,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>373</v>
-      </c>
       <c r="G13" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="14"/>
@@ -5116,20 +5112,20 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>374</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>377</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="27"/>
@@ -5138,25 +5134,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>326</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>328</v>
-      </c>
       <c r="G15" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="15"/>
@@ -5164,20 +5160,20 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>458</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>461</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
@@ -5186,10 +5182,10 @@
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D20" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.3">
@@ -5198,34 +5194,34 @@
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D22" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D23" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D24" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D25" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated plots and statistical tests
</commit_message>
<xml_diff>
--- a/IP/results/SummaryIP.xlsx
+++ b/IP/results/SummaryIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w63x712\Documents\Machine_Learning\HSI_selection2\IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AA4E82-1FAE-4EBD-8E34-DF1202748C7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31073FBE-7106-40F4-97B1-946DB80AB8FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{D4E1857A-7969-4B6E-A5E0-8AB94818FDA4}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="535">
   <si>
     <t>SVM</t>
   </si>
@@ -725,18 +725,6 @@
     <t>5 bands - Original</t>
   </si>
   <si>
-    <t>Ttest_relResult(statistic=7.3254933811136445, pvalue=4.4418847308318554e-05)</t>
-  </si>
-  <si>
-    <t>Ttest_relResult(statistic=5.755838895396393, pvalue=0.0002742723814363539)</t>
-  </si>
-  <si>
-    <t>Ttest_relResult(statistic=7.689516395167137, pvalue=3.032527136505947e-05)</t>
-  </si>
-  <si>
-    <t>Ttest_relResult(statistic=1.6880883097471708, pvalue=0.12566439774608748)</t>
-  </si>
-  <si>
     <t>5 bands - Gaussian transformation</t>
   </si>
   <si>
@@ -1629,6 +1617,36 @@
   </si>
   <si>
     <t>97.638% (+/- 0.952%)</t>
+  </si>
+  <si>
+    <t>print(stats.ttest_rel(df['GSS'], df['IBRA-PLS']))</t>
+  </si>
+  <si>
+    <t>print(stats.ttest_rel(df['GSS'], df['IBRA-PCA']))</t>
+  </si>
+  <si>
+    <t>Ttest_relResult(statistic=11.969998598081302, pvalue=7.865814775187436e-07)</t>
+  </si>
+  <si>
+    <t>Ttest_relResult(statistic=5.763012130352388, pvalue=0.0002718076949889121)</t>
+  </si>
+  <si>
+    <t>Ttest_relResult(statistic=7.699322009743164, pvalue=3.00208055292515e-05)</t>
+  </si>
+  <si>
+    <t>Ttest_relResult(statistic=5.006959201849547, pvalue=0.0007319846490779683)</t>
+  </si>
+  <si>
+    <t>Ttest_relResult(statistic=8.821368925015673, pvalue=1.0056640501770614e-05)</t>
+  </si>
+  <si>
+    <t>Ttest_relResult(statistic=3.2159829539590037, pvalue=0.010557153968696264)</t>
+  </si>
+  <si>
+    <t>Ttest_relResult(statistic=2.6940294639626434, pvalue=0.02463339877715231)</t>
+  </si>
+  <si>
+    <t>Ttest_relResult(statistic=3.2288191552156515, pvalue=0.010342194823020326)</t>
   </si>
 </sst>
 </file>
@@ -1848,98 +1866,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47677</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>151586</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1014597</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>68458</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7C26157-F5DC-4B65-BE62-B3AAA77463C1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="5734" t="9586" r="9011" b="5737"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="47677" y="3378880"/>
-          <a:ext cx="2620460" cy="1889107"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1222787</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>1795</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1331484</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>156197</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6EE624B-01D4-4C40-8DFA-74A4EC5993DC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6693947" y="3293635"/>
-          <a:ext cx="2874757" cy="2166082"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3066,7 +2992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448D17FE-18CC-46F5-BAC3-3C9188DFBB42}">
   <dimension ref="B3:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="107" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
@@ -3297,7 +3223,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -3328,16 +3254,16 @@
         <v>11</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -3348,16 +3274,16 @@
         <v>52</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
@@ -3368,16 +3294,16 @@
         <v>53</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
@@ -3388,16 +3314,16 @@
         <v>14</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
@@ -3408,16 +3334,16 @@
         <v>15</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
@@ -3428,16 +3354,16 @@
         <v>16</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
@@ -3448,16 +3374,16 @@
         <v>63</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
@@ -3468,16 +3394,16 @@
         <v>64</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
@@ -3502,7 +3428,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
@@ -3533,16 +3459,16 @@
         <v>11</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
@@ -3553,16 +3479,16 @@
         <v>52</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
@@ -3573,16 +3499,16 @@
         <v>53</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
@@ -3593,16 +3519,16 @@
         <v>14</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
@@ -3613,16 +3539,16 @@
         <v>15</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
@@ -3633,16 +3559,16 @@
         <v>16</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
@@ -3653,16 +3579,16 @@
         <v>63</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
@@ -3673,16 +3599,16 @@
         <v>64</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
@@ -3707,7 +3633,7 @@
         <v>3</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
@@ -3738,16 +3664,16 @@
         <v>11</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
@@ -3758,16 +3684,16 @@
         <v>12</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
@@ -3778,16 +3704,16 @@
         <v>53</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
@@ -3798,16 +3724,16 @@
         <v>14</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
@@ -3818,16 +3744,16 @@
         <v>15</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
@@ -3838,16 +3764,16 @@
         <v>16</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
@@ -3858,16 +3784,16 @@
         <v>63</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
@@ -3878,16 +3804,16 @@
         <v>64</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
@@ -3921,10 +3847,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D34A67-7EA1-4E46-B651-5814B8ED44C8}">
-  <dimension ref="A3:J38"/>
+  <dimension ref="A3:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3945,7 +3871,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4134,16 +4060,16 @@
         <v>156</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>185</v>
@@ -4158,16 +4084,16 @@
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="10" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G14" s="33"/>
       <c r="H14" s="34"/>
@@ -4194,7 +4120,7 @@
         <v>201</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="15"/>
@@ -4206,16 +4132,16 @@
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="11" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G16" s="33"/>
       <c r="H16" s="34"/>
@@ -4227,19 +4153,19 @@
         <v>151</v>
       </c>
       <c r="B17" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>461</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>462</v>
+      </c>
+      <c r="F17" s="22" t="s">
         <v>463</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>464</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>465</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>466</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -4248,16 +4174,16 @@
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="23" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -4265,19 +4191,19 @@
         <v>151</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -4286,16 +4212,16 @@
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="24" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -4303,7 +4229,7 @@
         <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C21">
         <v>94.31</v>
@@ -4312,7 +4238,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C22">
         <v>94.78</v>
@@ -4323,7 +4249,7 @@
         <v>153</v>
       </c>
       <c r="B23" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C23">
         <v>98.89</v>
@@ -4332,7 +4258,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="35"/>
       <c r="B24" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C24">
         <v>98.98</v>
@@ -4343,7 +4269,7 @@
         <v>226</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -4352,70 +4278,102 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D30" s="17" t="s">
-        <v>222</v>
+        <v>525</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>222</v>
+        <v>525</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D31" s="17" t="s">
-        <v>223</v>
+        <v>526</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>223</v>
+        <v>526</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D32" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D33" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D34" s="17"/>
-      <c r="I34" s="17"/>
+      <c r="D34" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D35" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D36" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>246</v>
-      </c>
+      <c r="D36" s="17"/>
+      <c r="I36" s="17"/>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D37" s="17" t="s">
-        <v>229</v>
+        <v>528</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>247</v>
+        <v>533</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D38" s="17" t="s">
-        <v>230</v>
+        <v>527</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>248</v>
+        <v>534</v>
+      </c>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D39" s="17" t="s">
+        <v>529</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D40" s="17" t="s">
+        <v>530</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D41" s="17" t="s">
+        <v>531</v>
+      </c>
+      <c r="I41" s="17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D42" s="17" t="s">
+        <v>532</v>
+      </c>
+      <c r="I42" s="17" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4439,7 +4397,6 @@
     <mergeCell ref="G9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4469,7 +4426,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4514,16 +4471,16 @@
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>162</v>
@@ -4538,16 +4495,16 @@
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="10" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="G8" s="31"/>
       <c r="H8" s="32"/>
@@ -4562,16 +4519,16 @@
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>164</v>
@@ -4586,16 +4543,16 @@
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="10" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="G10" s="31"/>
       <c r="H10" s="32"/>
@@ -4610,16 +4567,16 @@
         <v>155</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>163</v>
@@ -4634,16 +4591,16 @@
       </c>
       <c r="B12" s="26"/>
       <c r="C12" s="10" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="G12" s="31"/>
       <c r="H12" s="32"/>
@@ -4658,16 +4615,16 @@
         <v>156</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>185</v>
@@ -4682,16 +4639,16 @@
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="10" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G14" s="33"/>
       <c r="H14" s="34"/>
@@ -4706,19 +4663,19 @@
         <v>157</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="15"/>
@@ -4730,16 +4687,16 @@
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="11" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="G16" s="33"/>
       <c r="H16" s="34"/>
@@ -4751,19 +4708,19 @@
         <v>151</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -4772,16 +4729,16 @@
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="23" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -4789,19 +4746,19 @@
         <v>151</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -4810,19 +4767,19 @@
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="24" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -4936,7 +4893,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4981,16 +4938,16 @@
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>162</v>
@@ -5005,16 +4962,16 @@
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="10" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G8" s="31"/>
       <c r="H8" s="32"/>
@@ -5029,16 +4986,16 @@
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>164</v>
@@ -5053,16 +5010,16 @@
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="10" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="G10" s="31"/>
       <c r="H10" s="32"/>
@@ -5077,16 +5034,16 @@
         <v>155</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>163</v>
@@ -5101,16 +5058,16 @@
       </c>
       <c r="B12" s="26"/>
       <c r="C12" s="18" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G12" s="31"/>
       <c r="H12" s="32"/>
@@ -5125,16 +5082,16 @@
         <v>156</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>185</v>
@@ -5149,16 +5106,16 @@
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="10" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G14" s="33"/>
       <c r="H14" s="34"/>
@@ -5173,19 +5130,19 @@
         <v>157</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="15"/>
@@ -5197,16 +5154,16 @@
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="11" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G16" s="33"/>
       <c r="H16" s="34"/>
@@ -5218,19 +5175,19 @@
         <v>151</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -5239,16 +5196,16 @@
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="23" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -5256,19 +5213,19 @@
         <v>151</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -5277,19 +5234,19 @@
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="24" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -5403,7 +5360,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -5448,16 +5405,16 @@
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>162</v>
@@ -5472,16 +5429,16 @@
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="10" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G8" s="31"/>
       <c r="H8" s="32"/>
@@ -5496,16 +5453,16 @@
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>164</v>
@@ -5520,16 +5477,16 @@
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="10" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G10" s="31"/>
       <c r="H10" s="32"/>
@@ -5544,16 +5501,16 @@
         <v>155</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>163</v>
@@ -5568,16 +5525,16 @@
       </c>
       <c r="B12" s="26"/>
       <c r="C12" s="18" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="G12" s="31"/>
       <c r="H12" s="32"/>
@@ -5592,16 +5549,16 @@
         <v>156</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>185</v>
@@ -5616,16 +5573,16 @@
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="10" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G14" s="33"/>
       <c r="H14" s="34"/>
@@ -5640,19 +5597,19 @@
         <v>157</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="15"/>
@@ -5664,16 +5621,16 @@
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="11" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="G16" s="33"/>
       <c r="H16" s="34"/>
@@ -5685,19 +5642,19 @@
         <v>151</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -5706,16 +5663,16 @@
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="23" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -5723,19 +5680,19 @@
         <v>151</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -5744,19 +5701,19 @@
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="24" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added SR-SSIM for comparison
</commit_message>
<xml_diff>
--- a/IP/results/SummaryIP.xlsx
+++ b/IP/results/SummaryIP.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w63x712\Documents\Machine_Learning\HSI_selection2\IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31073FBE-7106-40F4-97B1-946DB80AB8FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE7127E-F32E-4C57-817D-FA9AF6006FCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{D4E1857A-7969-4B6E-A5E0-8AB94818FDA4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="4" activeTab="8" xr2:uid="{D4E1857A-7969-4B6E-A5E0-8AB94818FDA4}"/>
   </bookViews>
   <sheets>
     <sheet name="200 bands" sheetId="1" r:id="rId1"/>
     <sheet name="SVM 5 bands" sheetId="2" r:id="rId2"/>
     <sheet name="RF 5 bands" sheetId="5" r:id="rId3"/>
-    <sheet name="ANN 5 bands" sheetId="6" r:id="rId4"/>
-    <sheet name="CNN 5 bands" sheetId="3" r:id="rId5"/>
+    <sheet name="CNN 5 bands" sheetId="3" r:id="rId4"/>
+    <sheet name="ANN 5 bands" sheetId="6" r:id="rId5"/>
     <sheet name="Comparison" sheetId="7" r:id="rId6"/>
     <sheet name="Comparison 75%" sheetId="8" r:id="rId7"/>
     <sheet name="Comparison 50%" sheetId="9" r:id="rId8"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="569">
   <si>
     <t>SVM</t>
   </si>
@@ -1647,6 +1647,108 @@
   </si>
   <si>
     <t>Ttest_relResult(statistic=3.2288191552156515, pvalue=0.010342194823020326)</t>
+  </si>
+  <si>
+    <t>SR-SSIM</t>
+  </si>
+  <si>
+    <t>selection=[28, 52, 91, 104, 121]</t>
+  </si>
+  <si>
+    <t>97.282% (+/- 0.370%)</t>
+  </si>
+  <si>
+    <t>97.737% (+/- 0.436%)</t>
+  </si>
+  <si>
+    <t>97.341% (+/- 0.798%)</t>
+  </si>
+  <si>
+    <t>97.489% (+/- 0.565%)</t>
+  </si>
+  <si>
+    <t>96.825% (+/- 0.768%)</t>
+  </si>
+  <si>
+    <t>97.142% (+/- 1.024%)</t>
+  </si>
+  <si>
+    <t>96.816% (+/- 1.948%)</t>
+  </si>
+  <si>
+    <t>96.864% (+/- 1.470%)</t>
+  </si>
+  <si>
+    <t>95.134% (+/- 1.130%)</t>
+  </si>
+  <si>
+    <t>96.048% (+/- 0.962%)</t>
+  </si>
+  <si>
+    <t>95.520% (+/- 1.363%)</t>
+  </si>
+  <si>
+    <t>95.685% (+/- 1.113%)</t>
+  </si>
+  <si>
+    <t>94.559% (+/- 1.572%)</t>
+  </si>
+  <si>
+    <t>95.718% (+/- 1.249%)</t>
+  </si>
+  <si>
+    <t>95.498% (+/- 1.767%)</t>
+  </si>
+  <si>
+    <t>95.458% (+/- 1.516%)</t>
+  </si>
+  <si>
+    <t>90.371% (+/- 4.086%)</t>
+  </si>
+  <si>
+    <t>90.898% (+/- 5.190%)</t>
+  </si>
+  <si>
+    <t>89.965% (+/- 2.507%)</t>
+  </si>
+  <si>
+    <t>89.579% (+/- 4.287%)</t>
+  </si>
+  <si>
+    <t>89.649% (+/- 3.562%)</t>
+  </si>
+  <si>
+    <t>91.272% (+/- 3.458%)</t>
+  </si>
+  <si>
+    <t>90.914% (+/- 2.530%)</t>
+  </si>
+  <si>
+    <t>90.673% (+/- 3.216%)</t>
+  </si>
+  <si>
+    <t>82.436% (+/- 9.212%)</t>
+  </si>
+  <si>
+    <t>83.647% (+/- 8.709%)</t>
+  </si>
+  <si>
+    <t>79.401% (+/- 8.455%)</t>
+  </si>
+  <si>
+    <t>79.626% (+/- 9.247%)</t>
+  </si>
+  <si>
+    <t>81.866% (+/- 9.671%)</t>
+  </si>
+  <si>
+    <t>83.578% (+/- 8.916%)</t>
+  </si>
+  <si>
+    <t>78.789% (+/- 9.559%)</t>
+  </si>
+  <si>
+    <t>79.525% (+/- 10.585%)</t>
   </si>
 </sst>
 </file>
@@ -1691,15 +1793,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1744,12 +1852,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1817,8 +1951,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1835,19 +1993,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2484,10 +2646,10 @@
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="28"/>
       <c r="D18" t="s">
         <v>110</v>
       </c>
@@ -2723,10 +2885,10 @@
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="7" t="s">
         <v>87</v>
       </c>
@@ -2750,6 +2912,863 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448D17FE-18CC-46F5-BAC3-3C9188DFBB42}">
+  <dimension ref="B3:G72"/>
+  <sheetViews>
+    <sheetView zoomScale="107" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="54.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
+        <v>6</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
+        <v>5</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="9">
+        <v>12</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="9">
+        <v>11</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="4">
+        <v>9</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="9">
+        <v>8</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="9">
+        <v>7</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="9">
+        <v>6</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="9">
+        <v>5</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="28"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="9">
+        <v>12</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="9">
+        <v>11</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="4">
+        <v>10</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="3">
+        <v>9</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="9">
+        <v>8</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="9">
+        <v>7</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="9">
+        <v>6</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="9">
+        <v>5</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="28"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="9">
+        <v>12</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="9">
+        <v>11</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="3">
+        <v>10</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63" s="4">
+        <v>9</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B64" s="9">
+        <v>8</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B65" s="9">
+        <v>7</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B66" s="9">
+        <v>6</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B67" s="9">
+        <v>5</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B71" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B72" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C72" s="28"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B72:C72"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5EA16C-E0E1-4857-88AC-77E326AF1432}">
   <dimension ref="B3:G18"/>
   <sheetViews>
@@ -2962,10 +3981,10 @@
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="28"/>
       <c r="D18" t="s">
         <v>114</v>
       </c>
@@ -2988,869 +4007,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448D17FE-18CC-46F5-BAC3-3C9188DFBB42}">
-  <dimension ref="B3:G72"/>
-  <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="54.77734375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" customWidth="1"/>
-    <col min="6" max="6" width="20.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="4">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
-        <v>7</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>6</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
-        <v>5</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="9">
-        <v>12</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="9">
-        <v>11</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="3">
-        <v>10</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="4">
-        <v>9</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="9">
-        <v>8</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="9">
-        <v>7</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="9">
-        <v>6</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="9">
-        <v>5</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="9">
-        <v>12</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="9">
-        <v>11</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="4">
-        <v>10</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="3">
-        <v>9</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B46" s="9">
-        <v>8</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="9">
-        <v>7</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="9">
-        <v>6</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="9">
-        <v>5</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B57" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" s="20" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="9">
-        <v>12</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="9">
-        <v>11</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="3">
-        <v>10</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B63" s="4">
-        <v>9</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B64" s="9">
-        <v>8</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B65" s="9">
-        <v>7</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B66" s="9">
-        <v>6</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B67" s="9">
-        <v>5</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B71" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B72" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C72" s="25"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B72:C72"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D34A67-7EA1-4E46-B651-5814B8ED44C8}">
-  <dimension ref="A3:J42"/>
+  <dimension ref="A3:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37:I42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3875,22 +4037,22 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="26"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -3912,7 +4074,7 @@
       <c r="A7" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="34" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -3927,10 +4089,10 @@
       <c r="F7" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
@@ -3938,7 +4100,7 @@
       <c r="A8" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="10" t="s">
         <v>165</v>
       </c>
@@ -3951,8 +4113,8 @@
       <c r="F8" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
@@ -3960,7 +4122,7 @@
       <c r="A9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="34" t="s">
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -3975,10 +4137,10 @@
       <c r="F9" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="H9" s="32"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
@@ -3986,7 +4148,7 @@
       <c r="A10" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="10" t="s">
         <v>181</v>
       </c>
@@ -3999,8 +4161,8 @@
       <c r="F10" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
@@ -4008,7 +4170,7 @@
       <c r="A11" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="34" t="s">
         <v>155</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -4023,10 +4185,10 @@
       <c r="F11" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="32"/>
+      <c r="H11" s="30"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
@@ -4034,7 +4196,7 @@
       <c r="A12" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="26"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="10" t="s">
         <v>173</v>
       </c>
@@ -4047,347 +4209,385 @@
       <c r="F12" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="30"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="B13" s="40" t="s">
+        <v>535</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>537</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>538</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>539</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>540</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>536</v>
+      </c>
+      <c r="H13" s="44"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="41" t="s">
+        <v>541</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>542</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>544</v>
+      </c>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="H15" s="34"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="B15" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H15" s="32"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="34"/>
+      <c r="C16" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>459</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>462</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="H17" s="32"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>465</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>466</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="34"/>
+      <c r="C18" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="G18" s="31"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>492</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>518</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>519</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>461</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>462</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="24" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="23" t="s">
+        <v>464</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>465</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>466</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>492</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>518</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>519</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="24" t="s">
         <v>521</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D22" s="24" t="s">
         <v>522</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E22" s="24" t="s">
         <v>523</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F22" s="24" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="35" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="33" t="s">
         <v>151</v>
-      </c>
-      <c r="B21" t="s">
-        <v>457</v>
-      </c>
-      <c r="C21">
-        <v>94.31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
-      <c r="B22" t="s">
-        <v>458</v>
-      </c>
-      <c r="C22">
-        <v>94.78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="35" t="s">
-        <v>153</v>
       </c>
       <c r="B23" t="s">
         <v>457</v>
       </c>
       <c r="C23">
-        <v>98.89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+        <v>94.31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="33"/>
       <c r="B24" t="s">
         <v>458</v>
       </c>
       <c r="C24">
+        <v>94.78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" t="s">
+        <v>457</v>
+      </c>
+      <c r="C25">
+        <v>98.89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="33"/>
+      <c r="B26" t="s">
+        <v>458</v>
+      </c>
+      <c r="C26">
         <v>98.98</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D28" s="17" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D30" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="I28" s="17" t="s">
+      <c r="I30" s="17" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D29" s="17"/>
-      <c r="I29" s="17"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D30" s="17" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D31" s="17"/>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D32" s="17" t="s">
         <v>525</v>
       </c>
-      <c r="I30" s="17" t="s">
+      <c r="I32" s="17" t="s">
         <v>525</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D31" s="17" t="s">
-        <v>526</v>
-      </c>
-      <c r="I31" s="17" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D32" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="I32" s="17" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D33" s="17" t="s">
-        <v>223</v>
+        <v>526</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>223</v>
+        <v>526</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D34" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D35" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D36" s="17"/>
-      <c r="I36" s="17"/>
+      <c r="D36" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D37" s="17" t="s">
-        <v>528</v>
+        <v>225</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>533</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D38" s="17" t="s">
-        <v>527</v>
-      </c>
-      <c r="I38" s="17" t="s">
-        <v>534</v>
-      </c>
+      <c r="D38" s="17"/>
+      <c r="I38" s="17"/>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D39" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>241</v>
+        <v>533</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D40" s="17" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>242</v>
+        <v>534</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D41" s="17" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D42" s="17" t="s">
+        <v>530</v>
+      </c>
+      <c r="I42" s="17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D43" s="17" t="s">
+        <v>531</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D44" s="17" t="s">
         <v>532</v>
       </c>
-      <c r="I42" s="17" t="s">
+      <c r="I44" s="17" t="s">
         <v>244</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B19:B20"/>
+  <mergeCells count="19">
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="G5:J5"/>
@@ -4395,6 +4595,18 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="G7:H8"/>
     <mergeCell ref="G9:H10"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="G17:H18"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="G13:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4402,10 +4614,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91329088-2726-4B19-B800-EBB8BBF3C82A}">
-  <dimension ref="A3:J32"/>
+  <dimension ref="A3:J34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4430,22 +4642,22 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="26"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -4467,7 +4679,7 @@
       <c r="A7" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="34" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -4482,10 +4694,10 @@
       <c r="F7" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
@@ -4493,7 +4705,7 @@
       <c r="A8" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="10" t="s">
         <v>375</v>
       </c>
@@ -4506,8 +4718,8 @@
       <c r="F8" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
@@ -4515,7 +4727,7 @@
       <c r="A9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="34" t="s">
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4530,10 +4742,10 @@
       <c r="F9" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="H9" s="32"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
@@ -4541,7 +4753,7 @@
       <c r="A10" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="10" t="s">
         <v>399</v>
       </c>
@@ -4554,8 +4766,8 @@
       <c r="F10" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
@@ -4563,25 +4775,25 @@
       <c r="A11" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="26" t="s">
         <v>419</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="26" t="s">
         <v>420</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="26" t="s">
         <v>421</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="27" t="s">
         <v>422</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="32"/>
+      <c r="H11" s="30"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
@@ -4589,266 +4801,315 @@
       <c r="A12" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="26" t="s">
         <v>423</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="26" t="s">
         <v>424</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="26" t="s">
         <v>425</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="27" t="s">
         <v>426</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="30"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="B13" s="40" t="s">
+        <v>535</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>545</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>546</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>547</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>548</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>536</v>
+      </c>
+      <c r="H13" s="44"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="41" t="s">
+        <v>549</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>550</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>551</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>552</v>
+      </c>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="H15" s="34"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="B15" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H15" s="32"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>444</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>445</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>446</v>
-      </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="34"/>
+      <c r="C16" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>459</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>468</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>469</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>470</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="H17" s="32"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="23" t="s">
-        <v>472</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>473</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>474</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="34"/>
+      <c r="C18" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="G18" s="31"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>492</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>513</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>514</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>515</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>468</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>469</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="24" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="23" t="s">
+        <v>472</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>473</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>492</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>513</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>514</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>515</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="24" t="s">
         <v>509</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D22" s="24" t="s">
         <v>510</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E22" s="24" t="s">
         <v>511</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F22" s="24" t="s">
         <v>512</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I22" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D22" s="17" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D24" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I24" s="17" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D23" s="17"/>
-      <c r="I23" s="17" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D25" s="17"/>
+      <c r="I25" s="17" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D24" s="17" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D26" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I26" s="17" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D25" s="17" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D27" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I27" s="17" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D26" s="17" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D28" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D27" s="17" t="s">
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D29" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D28" s="17"/>
-      <c r="I28" s="17"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D29" s="17"/>
       <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D30" s="17"/>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D32" s="17"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="G9:H10"/>
     <mergeCell ref="B5:B6"/>
@@ -4858,10 +5119,11 @@
     <mergeCell ref="G7:H8"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G11:H12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="G13:H14"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="G15:H16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G17:H18"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4869,10 +5131,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E5C165-CC35-4B6C-959C-2E76B8D5E7AF}">
-  <dimension ref="A3:J32"/>
+  <dimension ref="A3:J34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4897,22 +5159,22 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="26"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -4934,7 +5196,7 @@
       <c r="A7" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="34" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -4949,10 +5211,10 @@
       <c r="F7" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
@@ -4960,7 +5222,7 @@
       <c r="A8" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="10" t="s">
         <v>383</v>
       </c>
@@ -4973,8 +5235,8 @@
       <c r="F8" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
@@ -4982,7 +5244,7 @@
       <c r="A9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="34" t="s">
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4997,10 +5259,10 @@
       <c r="F9" s="12" t="s">
         <v>406</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="H9" s="32"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
@@ -5008,7 +5270,7 @@
       <c r="A10" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="10" t="s">
         <v>407</v>
       </c>
@@ -5021,8 +5283,8 @@
       <c r="F10" s="12" t="s">
         <v>410</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
@@ -5030,7 +5292,7 @@
       <c r="A11" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="34" t="s">
         <v>155</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -5045,10 +5307,10 @@
       <c r="F11" s="19" t="s">
         <v>430</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="32"/>
+      <c r="H11" s="30"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
@@ -5056,7 +5318,7 @@
       <c r="A12" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="26"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="18" t="s">
         <v>431</v>
       </c>
@@ -5069,8 +5331,8 @@
       <c r="F12" s="19" t="s">
         <v>434</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="30"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
@@ -5078,244 +5340,296 @@
       <c r="A13" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>358</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="B13" s="40" t="s">
+        <v>535</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>553</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>554</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>555</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>556</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>536</v>
+      </c>
+      <c r="H13" s="44"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="41" t="s">
+        <v>557</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>558</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>559</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>560</v>
+      </c>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>346</v>
-      </c>
-      <c r="H15" s="34"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="B15" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H15" s="32"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="11" t="s">
-        <v>447</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>448</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="34"/>
+      <c r="C16" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>459</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>476</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>477</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>478</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>346</v>
+      </c>
+      <c r="H17" s="32"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="23" t="s">
-        <v>480</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>481</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>482</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="34"/>
+      <c r="C18" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="G18" s="31"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>492</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>501</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>502</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>503</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="24" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>482</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>492</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>501</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>502</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="24" t="s">
         <v>505</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D22" s="24" t="s">
         <v>506</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E22" s="24" t="s">
         <v>507</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F22" s="24" t="s">
         <v>508</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I22" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D22" s="17" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D24" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I24" s="17" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D23" s="17"/>
-      <c r="I23" s="17" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D25" s="17"/>
+      <c r="I25" s="17" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D24" s="17" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D26" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I26" s="17" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D25" s="17" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D27" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I27" s="17" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D26" s="17" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D28" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D27" s="17" t="s">
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D29" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D28" s="17"/>
-      <c r="I28" s="17"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D29" s="17"/>
       <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D30" s="17"/>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D32" s="17"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="G9:H10"/>
     <mergeCell ref="B5:B6"/>
@@ -5325,10 +5639,8 @@
     <mergeCell ref="G7:H8"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G11:H12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G17:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5336,10 +5648,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FC768F-9925-423C-8CB8-7B0AC8AB7AFE}">
-  <dimension ref="A3:J32"/>
+  <dimension ref="A3:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5364,22 +5676,22 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="26"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -5401,7 +5713,7 @@
       <c r="A7" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="34" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -5416,10 +5728,10 @@
       <c r="F7" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
@@ -5427,7 +5739,7 @@
       <c r="A8" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="10" t="s">
         <v>391</v>
       </c>
@@ -5440,8 +5752,8 @@
       <c r="F8" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
@@ -5449,7 +5761,7 @@
       <c r="A9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="34" t="s">
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -5464,10 +5776,10 @@
       <c r="F9" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="H9" s="32"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
@@ -5475,7 +5787,7 @@
       <c r="A10" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="10" t="s">
         <v>415</v>
       </c>
@@ -5488,8 +5800,8 @@
       <c r="F10" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
@@ -5497,7 +5809,7 @@
       <c r="A11" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="34" t="s">
         <v>155</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -5512,10 +5824,10 @@
       <c r="F11" s="19" t="s">
         <v>438</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="32"/>
+      <c r="H11" s="30"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
@@ -5523,7 +5835,7 @@
       <c r="A12" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="26"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="18" t="s">
         <v>439</v>
       </c>
@@ -5536,8 +5848,8 @@
       <c r="F12" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="30"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
@@ -5545,244 +5857,293 @@
       <c r="A13" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>363</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>366</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="B13" s="40" t="s">
+        <v>535</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>561</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>562</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>563</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>564</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>536</v>
+      </c>
+      <c r="H13" s="44"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="41" t="s">
+        <v>565</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>566</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>567</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>568</v>
+      </c>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="H15" s="34"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="B15" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H15" s="32"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="11" t="s">
-        <v>451</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>452</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>454</v>
-      </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="34"/>
+      <c r="C16" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>459</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>484</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>485</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>486</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="H17" s="32"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="23" t="s">
-        <v>488</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>489</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>490</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="34"/>
+      <c r="C18" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="G18" s="31"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>492</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>499</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>484</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>485</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>486</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="24" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="23" t="s">
+        <v>488</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>490</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>492</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>499</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="24" t="s">
         <v>493</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D22" s="24" t="s">
         <v>494</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E22" s="24" t="s">
         <v>495</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F22" s="24" t="s">
         <v>496</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I22" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D22" s="17" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D24" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I24" s="17" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D23" s="17"/>
-      <c r="I23" s="17" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D25" s="17"/>
+      <c r="I25" s="17" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D24" s="17" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D26" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I26" s="17" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D25" s="17" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D27" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I27" s="17" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D26" s="17" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D28" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D27" s="17" t="s">
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D29" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D28" s="17"/>
-      <c r="I28" s="17"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D29" s="17"/>
       <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D30" s="17"/>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D32" s="17"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="G9:H10"/>
     <mergeCell ref="B5:B6"/>
@@ -5792,10 +6153,11 @@
     <mergeCell ref="G7:H8"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G11:H12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="G13:H14"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="G15:H16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G17:H18"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed normalization for IBRA
</commit_message>
<xml_diff>
--- a/IP/results/SummaryIP.xlsx
+++ b/IP/results/SummaryIP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w63x712\Documents\Machine_Learning\HSI_selection2\IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49976DE-C37E-4FBC-991A-926605ECE7E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A93D4F-3419-414B-9304-034DB598942E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="37725" yWindow="2340" windowWidth="2100" windowHeight="585" activeTab="3" xr2:uid="{D4E1857A-7969-4B6E-A5E0-8AB94818FDA4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D4E1857A-7969-4B6E-A5E0-8AB94818FDA4}"/>
   </bookViews>
   <sheets>
     <sheet name="200 bands" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="569">
   <si>
     <t>SVM</t>
   </si>
@@ -1960,7 +1960,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1978,38 +2000,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2646,10 +2646,10 @@
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="31"/>
       <c r="D18" t="s">
         <v>110</v>
       </c>
@@ -2885,10 +2885,10 @@
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="7" t="s">
         <v>87</v>
       </c>
@@ -2915,8 +2915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448D17FE-18CC-46F5-BAC3-3C9188DFBB42}">
   <dimension ref="B3:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="107" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3124,10 +3124,10 @@
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="8" t="s">
         <v>218</v>
       </c>
@@ -3337,10 +3337,10 @@
       <c r="D35" s="6"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="C36" s="28"/>
+      <c r="C36" s="31"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -3542,10 +3542,10 @@
       <c r="D53" s="6"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="28" t="s">
+      <c r="B54" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="28"/>
+      <c r="C54" s="31"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
@@ -3747,10 +3747,10 @@
       <c r="D71" s="6"/>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B72" s="28" t="s">
+      <c r="B72" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="C72" s="28"/>
+      <c r="C72" s="31"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
@@ -3981,10 +3981,10 @@
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="31"/>
       <c r="D18" t="s">
         <v>114</v>
       </c>
@@ -4037,22 +4037,22 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="34"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -4074,7 +4074,7 @@
       <c r="A7" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="32" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -4089,10 +4089,10 @@
       <c r="F7" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="30"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
@@ -4100,7 +4100,7 @@
       <c r="A8" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="34"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="10" t="s">
         <v>165</v>
       </c>
@@ -4113,8 +4113,8 @@
       <c r="F8" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
@@ -4122,7 +4122,7 @@
       <c r="A9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4137,10 +4137,10 @@
       <c r="F9" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="H9" s="30"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
@@ -4148,7 +4148,7 @@
       <c r="A10" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="10" t="s">
         <v>181</v>
       </c>
@@ -4161,8 +4161,8 @@
       <c r="F10" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
@@ -4170,7 +4170,7 @@
       <c r="A11" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="32" t="s">
         <v>155</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -4185,10 +4185,10 @@
       <c r="F11" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="30"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
@@ -4196,7 +4196,7 @@
       <c r="A12" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="34"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="10" t="s">
         <v>173</v>
       </c>
@@ -4209,56 +4209,56 @@
       <c r="F12" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="30"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="42" t="s">
         <v>535</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="29" t="s">
         <v>537</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="29" t="s">
         <v>538</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="29" t="s">
         <v>539</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="30" t="s">
         <v>540</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="44" t="s">
         <v>536</v>
       </c>
-      <c r="H13" s="44"/>
+      <c r="H13" s="45"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="41" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="29" t="s">
         <v>541</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="29" t="s">
         <v>542</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="29" t="s">
         <v>543</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="30" t="s">
         <v>544</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
     </row>
@@ -4266,7 +4266,7 @@
       <c r="A15" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="32" t="s">
         <v>156</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -4281,10 +4281,10 @@
       <c r="F15" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="H15" s="32"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
     </row>
@@ -4292,7 +4292,7 @@
       <c r="A16" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="34"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="10" t="s">
         <v>232</v>
       </c>
@@ -4305,8 +4305,8 @@
       <c r="F16" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
     </row>
@@ -4314,7 +4314,7 @@
       <c r="A17" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="32" t="s">
         <v>157</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -4329,10 +4329,10 @@
       <c r="F17" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="H17" s="32"/>
+      <c r="H17" s="40"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
@@ -4340,7 +4340,7 @@
       <c r="A18" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="11" t="s">
         <v>237</v>
       </c>
@@ -4353,8 +4353,8 @@
       <c r="F18" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
     </row>
@@ -4362,7 +4362,7 @@
       <c r="A19" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="32" t="s">
         <v>459</v>
       </c>
       <c r="C19" s="22" t="s">
@@ -4382,7 +4382,7 @@
       <c r="A20" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="34"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="23" t="s">
         <v>464</v>
       </c>
@@ -4400,7 +4400,7 @@
       <c r="A21" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="32" t="s">
         <v>492</v>
       </c>
       <c r="C21" s="24" t="s">
@@ -4420,7 +4420,7 @@
       <c r="A22" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="34"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="24" t="s">
         <v>521</v>
       </c>
@@ -4435,7 +4435,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="41" t="s">
         <v>151</v>
       </c>
       <c r="B23" t="s">
@@ -4446,7 +4446,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="33"/>
+      <c r="A24" s="41"/>
       <c r="B24" t="s">
         <v>458</v>
       </c>
@@ -4455,7 +4455,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="41" t="s">
         <v>153</v>
       </c>
       <c r="B25" t="s">
@@ -4466,7 +4466,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="33"/>
+      <c r="A26" s="41"/>
       <c r="B26" t="s">
         <v>458</v>
       </c>
@@ -4588,13 +4588,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="G9:H10"/>
     <mergeCell ref="G11:H12"/>
     <mergeCell ref="G15:H16"/>
     <mergeCell ref="G17:H18"/>
@@ -4607,6 +4600,13 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="G13:H14"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="G9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4642,22 +4642,22 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="34"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -4679,7 +4679,7 @@
       <c r="A7" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="32" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -4694,10 +4694,10 @@
       <c r="F7" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="30"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
@@ -4705,7 +4705,7 @@
       <c r="A8" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="34"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="10" t="s">
         <v>375</v>
       </c>
@@ -4718,8 +4718,8 @@
       <c r="F8" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
@@ -4727,7 +4727,7 @@
       <c r="A9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4742,10 +4742,10 @@
       <c r="F9" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="H9" s="30"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
@@ -4753,7 +4753,7 @@
       <c r="A10" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="10" t="s">
         <v>399</v>
       </c>
@@ -4766,8 +4766,8 @@
       <c r="F10" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
@@ -4775,7 +4775,7 @@
       <c r="A11" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="32" t="s">
         <v>155</v>
       </c>
       <c r="C11" s="26" t="s">
@@ -4790,10 +4790,10 @@
       <c r="F11" s="27" t="s">
         <v>422</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="30"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
@@ -4801,7 +4801,7 @@
       <c r="A12" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="34"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="26" t="s">
         <v>423</v>
       </c>
@@ -4814,56 +4814,56 @@
       <c r="F12" s="27" t="s">
         <v>426</v>
       </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="30"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="42" t="s">
         <v>535</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="29" t="s">
         <v>545</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="29" t="s">
         <v>546</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="29" t="s">
         <v>547</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="30" t="s">
         <v>548</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="44" t="s">
         <v>536</v>
       </c>
-      <c r="H13" s="44"/>
+      <c r="H13" s="45"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="41" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="29" t="s">
         <v>549</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="29" t="s">
         <v>550</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="29" t="s">
         <v>551</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="30" t="s">
         <v>552</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
     </row>
@@ -4871,7 +4871,7 @@
       <c r="A15" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="32" t="s">
         <v>156</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -4886,10 +4886,10 @@
       <c r="F15" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="H15" s="32"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
     </row>
@@ -4897,7 +4897,7 @@
       <c r="A16" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="34"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="10" t="s">
         <v>351</v>
       </c>
@@ -4910,8 +4910,8 @@
       <c r="F16" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
     </row>
@@ -4919,7 +4919,7 @@
       <c r="A17" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="32" t="s">
         <v>157</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -4934,10 +4934,10 @@
       <c r="F17" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="H17" s="32"/>
+      <c r="H17" s="40"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
@@ -4945,7 +4945,7 @@
       <c r="A18" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="11" t="s">
         <v>443</v>
       </c>
@@ -4958,8 +4958,8 @@
       <c r="F18" s="13" t="s">
         <v>446</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
     </row>
@@ -4967,7 +4967,7 @@
       <c r="A19" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="32" t="s">
         <v>459</v>
       </c>
       <c r="C19" s="23" t="s">
@@ -4987,7 +4987,7 @@
       <c r="A20" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="34"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="23" t="s">
         <v>472</v>
       </c>
@@ -5005,7 +5005,7 @@
       <c r="A21" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="32" t="s">
         <v>492</v>
       </c>
       <c r="C21" s="24" t="s">
@@ -5025,7 +5025,7 @@
       <c r="A22" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="34"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="24" t="s">
         <v>509</v>
       </c>
@@ -5107,16 +5107,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="G7:H8"/>
     <mergeCell ref="G13:H14"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="G9:H10"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="G7:H8"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G11:H12"/>
     <mergeCell ref="B15:B16"/>
@@ -5159,22 +5159,22 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="34"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -5196,7 +5196,7 @@
       <c r="A7" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="32" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -5211,10 +5211,10 @@
       <c r="F7" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="30"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
@@ -5222,7 +5222,7 @@
       <c r="A8" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="34"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="10" t="s">
         <v>383</v>
       </c>
@@ -5235,8 +5235,8 @@
       <c r="F8" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
@@ -5244,7 +5244,7 @@
       <c r="A9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -5259,10 +5259,10 @@
       <c r="F9" s="12" t="s">
         <v>406</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="H9" s="30"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
@@ -5270,7 +5270,7 @@
       <c r="A10" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="10" t="s">
         <v>407</v>
       </c>
@@ -5283,8 +5283,8 @@
       <c r="F10" s="12" t="s">
         <v>410</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
@@ -5292,7 +5292,7 @@
       <c r="A11" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="32" t="s">
         <v>155</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -5307,10 +5307,10 @@
       <c r="F11" s="19" t="s">
         <v>430</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="30"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
@@ -5318,7 +5318,7 @@
       <c r="A12" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="34"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="18" t="s">
         <v>431</v>
       </c>
@@ -5331,8 +5331,8 @@
       <c r="F12" s="19" t="s">
         <v>434</v>
       </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="30"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
@@ -5340,25 +5340,25 @@
       <c r="A13" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="42" t="s">
         <v>535</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="29" t="s">
         <v>553</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="29" t="s">
         <v>554</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="29" t="s">
         <v>555</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="44" t="s">
         <v>536</v>
       </c>
-      <c r="H13" s="44"/>
+      <c r="H13" s="45"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
     </row>
@@ -5366,21 +5366,21 @@
       <c r="A14" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="41" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="29" t="s">
         <v>557</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="29" t="s">
         <v>558</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="29" t="s">
         <v>559</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="30" t="s">
         <v>560</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
     </row>
@@ -5388,7 +5388,7 @@
       <c r="A15" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="32" t="s">
         <v>156</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -5403,10 +5403,10 @@
       <c r="F15" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="H15" s="32"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
     </row>
@@ -5414,7 +5414,7 @@
       <c r="A16" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="34"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="10" t="s">
         <v>359</v>
       </c>
@@ -5427,8 +5427,8 @@
       <c r="F16" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
     </row>
@@ -5436,7 +5436,7 @@
       <c r="A17" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="32" t="s">
         <v>157</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -5451,10 +5451,10 @@
       <c r="F17" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="39" t="s">
         <v>346</v>
       </c>
-      <c r="H17" s="32"/>
+      <c r="H17" s="40"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
@@ -5462,7 +5462,7 @@
       <c r="A18" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="11" t="s">
         <v>447</v>
       </c>
@@ -5475,8 +5475,8 @@
       <c r="F18" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
     </row>
@@ -5484,7 +5484,7 @@
       <c r="A19" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="32" t="s">
         <v>459</v>
       </c>
       <c r="C19" s="23" t="s">
@@ -5504,7 +5504,7 @@
       <c r="A20" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="34"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="23" t="s">
         <v>480</v>
       </c>
@@ -5522,7 +5522,7 @@
       <c r="A21" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="32" t="s">
         <v>492</v>
       </c>
       <c r="C21" s="24" t="s">
@@ -5542,7 +5542,7 @@
       <c r="A22" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="34"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="24" t="s">
         <v>505</v>
       </c>
@@ -5624,12 +5624,10 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G17:H18"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="G9:H10"/>
     <mergeCell ref="B5:B6"/>
@@ -5637,10 +5635,12 @@
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="G7:H8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="G17:H18"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B19:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5676,22 +5676,22 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="34"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -5713,7 +5713,7 @@
       <c r="A7" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="32" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -5728,10 +5728,10 @@
       <c r="F7" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="30"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
@@ -5739,7 +5739,7 @@
       <c r="A8" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="34"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="10" t="s">
         <v>391</v>
       </c>
@@ -5752,8 +5752,8 @@
       <c r="F8" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
@@ -5761,7 +5761,7 @@
       <c r="A9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -5776,10 +5776,10 @@
       <c r="F9" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="H9" s="30"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
@@ -5787,7 +5787,7 @@
       <c r="A10" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="10" t="s">
         <v>415</v>
       </c>
@@ -5800,8 +5800,8 @@
       <c r="F10" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
@@ -5809,7 +5809,7 @@
       <c r="A11" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="32" t="s">
         <v>155</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -5824,10 +5824,10 @@
       <c r="F11" s="19" t="s">
         <v>438</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="30"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
@@ -5835,7 +5835,7 @@
       <c r="A12" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="34"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="18" t="s">
         <v>439</v>
       </c>
@@ -5848,8 +5848,8 @@
       <c r="F12" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="30"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
@@ -5857,25 +5857,25 @@
       <c r="A13" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="42" t="s">
         <v>535</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="29" t="s">
         <v>561</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="29" t="s">
         <v>562</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="29" t="s">
         <v>563</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="30" t="s">
         <v>564</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="44" t="s">
         <v>536</v>
       </c>
-      <c r="H13" s="44"/>
+      <c r="H13" s="45"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
     </row>
@@ -5883,21 +5883,21 @@
       <c r="A14" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="41" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="29" t="s">
         <v>565</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="29" t="s">
         <v>566</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="29" t="s">
         <v>567</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="30" t="s">
         <v>568</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
     </row>
@@ -5905,7 +5905,7 @@
       <c r="A15" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="32" t="s">
         <v>156</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -5920,10 +5920,10 @@
       <c r="F15" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="H15" s="32"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
     </row>
@@ -5931,7 +5931,7 @@
       <c r="A16" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="34"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="10" t="s">
         <v>367</v>
       </c>
@@ -5944,8 +5944,8 @@
       <c r="F16" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
     </row>
@@ -5953,7 +5953,7 @@
       <c r="A17" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="32" t="s">
         <v>157</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -5968,10 +5968,10 @@
       <c r="F17" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="H17" s="32"/>
+      <c r="H17" s="40"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
@@ -5979,7 +5979,7 @@
       <c r="A18" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="11" t="s">
         <v>451</v>
       </c>
@@ -5992,8 +5992,8 @@
       <c r="F18" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
     </row>
@@ -6001,7 +6001,7 @@
       <c r="A19" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="32" t="s">
         <v>459</v>
       </c>
       <c r="C19" s="23" t="s">
@@ -6021,7 +6021,7 @@
       <c r="A20" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="34"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="23" t="s">
         <v>488</v>
       </c>
@@ -6039,7 +6039,7 @@
       <c r="A21" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="32" t="s">
         <v>492</v>
       </c>
       <c r="C21" s="24" t="s">
@@ -6059,7 +6059,7 @@
       <c r="A22" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="34"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="24" t="s">
         <v>493</v>
       </c>
@@ -6141,16 +6141,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="G7:H8"/>
     <mergeCell ref="G13:H14"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="G9:H10"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="G7:H8"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G11:H12"/>
     <mergeCell ref="B15:B16"/>

</xml_diff>